<commit_message>
updated Model tuning results file in Capstone
</commit_message>
<xml_diff>
--- a/Capstone/Model_Tuning_Results.xlsx
+++ b/Capstone/Model_Tuning_Results.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>model</t>
   </si>
@@ -44,91 +45,103 @@
     <t>holdout score</t>
   </si>
   <si>
-    <t>max_depth = None</t>
-  </si>
-  <si>
-    <t>min_samples_leaf=1</t>
-  </si>
-  <si>
-    <t>n_estimators=150</t>
-  </si>
-  <si>
-    <t>max_features=1/3</t>
-  </si>
-  <si>
-    <t>min_samples_leaf=5</t>
-  </si>
-  <si>
     <t>score_diff</t>
   </si>
   <si>
-    <t>[None]</t>
-  </si>
-  <si>
-    <t>[1,3,5,7]</t>
-  </si>
-  <si>
-    <t>np.arange(25,151,25)</t>
-  </si>
-  <si>
-    <t>[1/3,None]</t>
-  </si>
-  <si>
     <t>EN</t>
   </si>
   <si>
-    <t>alpha=0.01</t>
-  </si>
-  <si>
-    <t>fit_intercept=True</t>
-  </si>
-  <si>
-    <t>l1_ratio=0.01</t>
-  </si>
-  <si>
-    <t>[.001,.01,.1,1,10]</t>
-  </si>
-  <si>
-    <t>[True,False]</t>
-  </si>
-  <si>
-    <t>[.01,.05,1,.25,.5,.8,.9]</t>
-  </si>
-  <si>
     <t>GBT</t>
   </si>
   <si>
-    <t>learning_rate=0.05</t>
-  </si>
-  <si>
-    <t>max_depth=5</t>
-  </si>
-  <si>
-    <t>max_features=None</t>
-  </si>
-  <si>
-    <t>subsample=0.8</t>
-  </si>
-  <si>
-    <t>max_depth=3</t>
-  </si>
-  <si>
-    <t>n_estimators=200</t>
-  </si>
-  <si>
-    <t>subsample=0.5</t>
-  </si>
-  <si>
-    <t>[3,5,7,9]</t>
-  </si>
-  <si>
-    <t>[100,150,200]</t>
-  </si>
-  <si>
-    <t>[0.5,0.8,1.0]</t>
-  </si>
-  <si>
-    <t>[0.05,0.1,0.3]</t>
+    <t>RF grid</t>
+  </si>
+  <si>
+    <t>EN grid</t>
+  </si>
+  <si>
+    <t>GBT grid</t>
+  </si>
+  <si>
+    <t>Kneighbors</t>
+  </si>
+  <si>
+    <t>Kneighbors grid</t>
+  </si>
+  <si>
+    <t>SVM grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM </t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>max_depth: [None]</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>min_samples_leaf: [1,3,5,7]</t>
+  </si>
+  <si>
+    <t>n_estimators: np.arange(25,151,25)</t>
+  </si>
+  <si>
+    <t>max_features: [1/3,None]</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>alpha: [.001,.01,.1,1,10]</t>
+  </si>
+  <si>
+    <t>fit_intercept: [True,False]</t>
+  </si>
+  <si>
+    <t>l1_ratio: [.01,.05,1,.25,.5,.8,.9]</t>
+  </si>
+  <si>
+    <t>learning_rate: [0.05,0.1,0.3]</t>
+  </si>
+  <si>
+    <t>max_depth: [3,5,7,9]</t>
+  </si>
+  <si>
+    <t>n_estimators: [100,150,200]</t>
+  </si>
+  <si>
+    <t>subsample: [0.5,0.8,1.0]</t>
+  </si>
+  <si>
+    <t>n_neighrbors: np.arange(3,22,2)</t>
+  </si>
+  <si>
+    <t>kernel: [linear,rbf,poly]</t>
+  </si>
+  <si>
+    <t>degree: [2,3,4]</t>
+  </si>
+  <si>
+    <t>gamma: [auto,0.1,1,10]</t>
+  </si>
+  <si>
+    <t>C: [0.1,1,10]</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>epsilon: [0.05,0.1,0.2,0.4]</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>NN</t>
   </si>
 </sst>
 </file>
@@ -164,10 +177,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,18 +505,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
@@ -508,13 +529,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" t="s">
         <v>3</v>
       </c>
@@ -522,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -530,45 +551,49 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>150</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
         <v>0.15640000000000001</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>0.3952</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <f>ABS(H3-G3)</f>
         <v>0.23879999999999998</v>
       </c>
@@ -577,167 +602,286 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>150</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>0.33229999999999998</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>0.40029999999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <f>ABS(H4-G4)</f>
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
         <v>0.4143</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0.4163</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I12" si="0">ABS(H6-G6)</f>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I14" si="0">ABS(H6-G6)</f>
         <v>2.0000000000000018E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8">
+      <c r="B8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <v>150</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.29270000000000002</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>0.40529999999999999</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>0.11259999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1">
+        <v>200</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.36749999999999999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>0.4078</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>0.43280000000000002</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.4365</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I11">
+        <v>3.6999999999999811E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.40339999999999998</v>
+      </c>
+      <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I12">
+        <v>0.10259999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.37769999999999998</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.41260000000000002</v>
+      </c>
+      <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4900000000000042E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -745,5 +889,6 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added newest games and changed train/test split to 80/20
</commit_message>
<xml_diff>
--- a/Capstone/Model_Tuning_Results.xlsx
+++ b/Capstone/Model_Tuning_Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -508,7 +507,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,14 +587,17 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1">
-        <v>0.15640000000000001</v>
+        <v>0.1215</v>
       </c>
       <c r="H3" s="1">
-        <v>0.3952</v>
+        <v>0.31630000000000003</v>
       </c>
       <c r="I3" s="1">
         <f>ABS(H3-G3)</f>
-        <v>0.23879999999999998</v>
+        <v>0.19480000000000003</v>
+      </c>
+      <c r="J3">
+        <v>0.30430000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>